<commit_message>
Se agrego la carpeta SHS a la carpeta Linea Base y se actualizo el cronograma
</commit_message>
<xml_diff>
--- a/Desarrollo/SHS/Gestión/SHS-CP.xlsx
+++ b/Desarrollo/SHS/Gestión/SHS-CP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Jose Tirado\OneDrive\Escritorio\6to ciclo\ProyectoGestionConfig\ServiceHomeStore\Desarrollo\SHS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Jose Tirado\OneDrive\Escritorio\6to ciclo\ProyectoGestionConfig\ServiceHomeStore\Desarrollo\SHS\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE4062D-3D8D-4500-9207-B668D8AB9195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A9B859-0B05-40A4-90E8-C26346D6862A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="124">
   <si>
     <t>CRONOGRAMA DEL PROYECTO</t>
   </si>
@@ -129,9 +129,6 @@
     <t>Elaboración de la especificación del requisito 01: Login</t>
   </si>
   <si>
-    <t>Alvarado(Bk), Cortez(Ft),Quinteros(Fs)</t>
-  </si>
-  <si>
     <t>Elaboración de la especificación del requisito 02:Agregar servicios</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>Elaboración de la especificación del requisito 03:Editar servicios</t>
   </si>
   <si>
-    <t>Aquino(Ft),  Maita(Ft)</t>
-  </si>
-  <si>
     <t>Elaboración de la especificación del requisito 04:Borrar servicios</t>
   </si>
   <si>
@@ -159,54 +153,21 @@
     <t>Elaboración de la especificación del requisito 07: Editar perfil del usuario</t>
   </si>
   <si>
-    <t>Tirado(Jp), Aquino(Ft), Quintero(Fs)</t>
-  </si>
-  <si>
     <t>Elaboración de la especificación del requisito 08: Eliminar cuenta</t>
   </si>
   <si>
-    <t>Alberto(Ft), Rojas(Bk)</t>
-  </si>
-  <si>
     <t>Elaboración de la especificación del requisito 09: Gestion de servicios</t>
   </si>
   <si>
-    <t>Maita(Ft), Frank(Bk), Rojas(Bk)</t>
-  </si>
-  <si>
-    <t>Elaboración de la especificación del requisito 010: Seccion de busqueda de servicio</t>
-  </si>
-  <si>
-    <t>Alberto(Ft),Cortez(Ft)</t>
-  </si>
-  <si>
-    <t>Elaboración de la especificación del requisito 011: Seccion de discusión en los servicios</t>
-  </si>
-  <si>
-    <t>Quinteros(Fs), Rojas(Bk), Tirado(Jp)</t>
-  </si>
-  <si>
-    <t>Elaboración de la especificación del requisito 012: Adquirir servicios</t>
-  </si>
-  <si>
-    <t>Cortez(Ft),Quinteros(Fs),Tirado(Jp)</t>
-  </si>
-  <si>
     <t>Elaborar Documento de analisis</t>
   </si>
   <si>
     <t>Elaborar diagramas de actividades</t>
   </si>
   <si>
-    <t>Aquino(Ft), Alvarado(Bk), Tirado(Jp)</t>
-  </si>
-  <si>
     <t>Elaborar diagramas de casos de uso</t>
   </si>
   <si>
-    <t>CortezFs)</t>
-  </si>
-  <si>
     <t>Elaborar prototipos</t>
   </si>
   <si>
@@ -249,9 +210,6 @@
     <t>Creacion de la tabla servicios</t>
   </si>
   <si>
-    <t>Codificacion:</t>
-  </si>
-  <si>
     <t>Desarrollo frontend</t>
   </si>
   <si>
@@ -354,9 +312,6 @@
     <t>Alvarado(Bk),Quinteros(Fs), Tirado(Jp)</t>
   </si>
   <si>
-    <t>Hito #4 :11/01/2020</t>
-  </si>
-  <si>
     <t>Ayuda al usuario:</t>
   </si>
   <si>
@@ -385,6 +340,63 @@
   </si>
   <si>
     <t>Alvarado(Ft),Aquino(Ft),Cortez(Ft),Quinteros(Fs), Tirado(Jp)</t>
+  </si>
+  <si>
+    <t>Elaboración de la especificación del requisito 10: Seccion de busqueda de servicio</t>
+  </si>
+  <si>
+    <t>Elaboración de la especificación del requisito 11: Seccion de discusión en los servicios</t>
+  </si>
+  <si>
+    <t>Elaboración de la especificación del requisito 12: Adquirir servicios</t>
+  </si>
+  <si>
+    <t>Alberto(Ft),Rojas(Bk),Tirado(Jp)</t>
+  </si>
+  <si>
+    <t>Maita(Ft),Quinteros(Fs), Rojas(Bk)</t>
+  </si>
+  <si>
+    <t>Aquino(Ft),Cortez(Ft),Quinteros(Fs),</t>
+  </si>
+  <si>
+    <t>Alberto(Ft),Cortez(Ft),Tirado(Jp)</t>
+  </si>
+  <si>
+    <t>Alvarado(Bk),Maita(Ft), Rojas(Bk)</t>
+  </si>
+  <si>
+    <t>Alberto(Ft), Alvarado(Bk), Rojas(Bk)</t>
+  </si>
+  <si>
+    <t>Alberto(Ft),Alvarado(Bk), Maita(Ft)</t>
+  </si>
+  <si>
+    <t>Aquino(Ft), Cortez(Ft),Rojas(Bk)</t>
+  </si>
+  <si>
+    <t>Alberto(Ft),Aquino(Ft),  Maita(Ft)</t>
+  </si>
+  <si>
+    <t>Aquino(Ft),Cortez(Ft),Quinteros(Fs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aquino(Ft) </t>
+  </si>
+  <si>
+    <t>Alberto(Ft)</t>
+  </si>
+  <si>
+    <t>Aquino(Ft),Quinteros(Fs),Tirado(Jp)</t>
+  </si>
+  <si>
+    <t>Cortez(Ft)</t>
+  </si>
+  <si>
+    <t>Hito #4 :19/01/2020</t>
+  </si>
+  <si>
+    <t>Codificacion</t>
   </si>
 </sst>
 </file>
@@ -394,7 +406,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,17 +463,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <i/>
       <sz val="11"/>
@@ -472,6 +473,51 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -495,7 +541,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -522,36 +568,27 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top style="thin">
+      <right style="thin">
         <color rgb="FF000000"/>
-      </top>
+      </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,17 +599,61 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top/>
-      <bottom style="thin">
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color rgb="FF000000"/>
-      </bottom>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -594,34 +675,30 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -638,12 +715,33 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -861,8 +959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="S47" sqref="S47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -877,46 +975,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:34" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
+      <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="36"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
@@ -936,67 +1034,67 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="36"/>
-      <c r="P3" s="36"/>
-      <c r="Q3" s="36"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
+      <c r="Q3" s="32"/>
     </row>
     <row r="4" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="35">
         <v>44132</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="32"/>
     </row>
     <row r="5" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="36">
         <v>44216</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
-      <c r="O5" s="36"/>
-      <c r="P5" s="36"/>
-      <c r="Q5" s="36"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="32"/>
     </row>
     <row r="6" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -1131,77 +1229,77 @@
       </c>
     </row>
     <row r="10" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="10" t="s">
+      <c r="C10" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q10" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="43"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="54"/>
+      <c r="N11" s="54"/>
+      <c r="O11" s="54"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
     </row>
     <row r="12" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
     </row>
     <row r="13" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="6"/>
@@ -1220,15 +1318,15 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="10" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="Q13" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B14" s="14" t="s">
-        <v>35</v>
+      <c r="B14" s="13" t="s">
+        <v>34</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1246,15 +1344,15 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q14" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
-        <v>37</v>
+      <c r="B15" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1274,15 +1372,15 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="10" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="Q15" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B16" s="15" t="s">
-        <v>39</v>
+      <c r="B16" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1302,15 +1400,15 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="10" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="Q16" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B17" s="14" t="s">
-        <v>40</v>
+      <c r="B17" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1330,15 +1428,15 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q17" s="16">
+        <v>120</v>
+      </c>
+      <c r="Q17" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B18" s="14" t="s">
-        <v>42</v>
+      <c r="B18" s="13" t="s">
+        <v>40</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -1358,15 +1456,15 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="10" t="s">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="Q18" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:17" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B19" s="14" t="s">
-        <v>43</v>
+      <c r="B19" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1375,24 +1473,24 @@
       <c r="G19" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H19" s="17"/>
+      <c r="H19" s="16"/>
       <c r="I19" s="6"/>
-      <c r="J19" s="12"/>
+      <c r="J19" s="11"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="10" t="s">
-        <v>44</v>
+        <v>108</v>
       </c>
       <c r="Q19" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
-        <v>45</v>
+      <c r="B20" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -1410,15 +1508,15 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="10" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="Q20" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="15" t="s">
-        <v>47</v>
+      <c r="B21" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1436,15 +1534,15 @@
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="10" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="Q21" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>49</v>
+      <c r="B22" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1462,15 +1560,15 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="10" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="Q22" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
-        <v>51</v>
+      <c r="B23" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1479,8 +1577,8 @@
       <c r="G23" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -1488,15 +1586,15 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="9" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="Q23" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="14" t="s">
-        <v>53</v>
+      <c r="B24" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1506,7 +1604,7 @@
         <v>25</v>
       </c>
       <c r="H24" s="9"/>
-      <c r="I24" s="12"/>
+      <c r="I24" s="11"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -1514,15 +1612,15 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="10" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="Q24" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="18" t="s">
-        <v>55</v>
+      <c r="B25" s="17" t="s">
+        <v>44</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1530,8 +1628,8 @@
       <c r="F25" s="6"/>
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
@@ -1542,7 +1640,7 @@
     </row>
     <row r="26" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1552,15 +1650,15 @@
       <c r="H26" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="10" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="Q26" s="7">
         <v>1</v>
@@ -1568,7 +1666,7 @@
     </row>
     <row r="27" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1580,85 +1678,85 @@
       </c>
       <c r="I27" s="9"/>
       <c r="J27" s="6"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
       <c r="M27" s="6"/>
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="10" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="Q27" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+      <c r="B28" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
       <c r="H28" s="9" t="s">
         <v>25</v>
       </c>
       <c r="I28" s="9"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
       <c r="L28" s="9"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="44" t="s">
-        <v>61</v>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="30" t="s">
+        <v>48</v>
       </c>
       <c r="Q28" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
+      <c r="B29" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-      <c r="N29" s="19"/>
-      <c r="O29" s="19"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="7"/>
     </row>
     <row r="30" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+        <v>51</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
       <c r="H30" s="9" t="s">
         <v>25</v>
       </c>
       <c r="I30" s="9"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
       <c r="P30" s="10" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="Q30" s="7">
         <v>1</v>
@@ -1666,17 +1764,17 @@
     </row>
     <row r="31" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-      <c r="H31" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I31" s="17"/>
+      <c r="H31" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I31" s="16"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="6"/>
@@ -1684,99 +1782,99 @@
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="9" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="Q31" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" s="21"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-      <c r="N32" s="19"/>
-      <c r="O32" s="19"/>
-      <c r="P32" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q32" s="7">
+      <c r="B32" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="40"/>
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q32" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-      <c r="N33" s="19"/>
-      <c r="O33" s="19"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="7"/>
+      <c r="B33" s="51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="51"/>
+      <c r="F33" s="51"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="51"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="51"/>
+      <c r="K33" s="51"/>
+      <c r="L33" s="51"/>
+      <c r="M33" s="51"/>
+      <c r="N33" s="51"/>
+      <c r="O33" s="51"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51"/>
     </row>
     <row r="34" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="7"/>
+      <c r="B34" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="29"/>
     </row>
     <row r="35" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
+        <v>59</v>
+      </c>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-      <c r="N35" s="19"/>
-      <c r="O35" s="19"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
+      <c r="N35" s="18"/>
+      <c r="O35" s="18"/>
       <c r="P35" s="9" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="Q35" s="7">
         <v>1</v>
@@ -1784,41 +1882,41 @@
     </row>
     <row r="36" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
+        <v>60</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
       <c r="I36" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="18"/>
+      <c r="O36" s="18"/>
       <c r="P36" s="9" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="Q36" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="19"/>
-      <c r="D37" s="19"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="19"/>
-      <c r="H37" s="19"/>
-      <c r="I37" s="17"/>
+      <c r="B37" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="16"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="6"/>
@@ -1829,46 +1927,46 @@
       <c r="Q37" s="7"/>
     </row>
     <row r="38" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="C38" s="19"/>
-      <c r="D38" s="19"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="21"/>
+      <c r="B38" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C38" s="18"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="18"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="20"/>
       <c r="J38" s="9"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
+      <c r="K38" s="18"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="18"/>
+      <c r="N38" s="18"/>
+      <c r="O38" s="18"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="7"/>
     </row>
     <row r="39" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="19"/>
-      <c r="D39" s="19"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="19"/>
+        <v>62</v>
+      </c>
+      <c r="C39" s="18"/>
+      <c r="D39" s="18"/>
+      <c r="E39" s="18"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18"/>
       <c r="H39" s="9"/>
-      <c r="I39" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="J39" s="17"/>
+      <c r="I39" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="J39" s="16"/>
       <c r="K39" s="9"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
       <c r="P39" s="9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="Q39" s="7">
         <v>1</v>
@@ -1876,25 +1974,25 @@
     </row>
     <row r="40" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C40" s="19"/>
-      <c r="D40" s="19"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
+        <v>63</v>
+      </c>
+      <c r="C40" s="18"/>
+      <c r="D40" s="18"/>
+      <c r="E40" s="18"/>
+      <c r="F40" s="18"/>
+      <c r="G40" s="18"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="J40" s="21"/>
+      <c r="J40" s="20"/>
       <c r="K40" s="9"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
       <c r="P40" s="9" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="Q40" s="7">
         <v>1</v>
@@ -1902,25 +2000,25 @@
     </row>
     <row r="41" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C41" s="19"/>
-      <c r="D41" s="19"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
+        <v>65</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="18"/>
+      <c r="E41" s="18"/>
+      <c r="F41" s="18"/>
+      <c r="G41" s="18"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9" t="s">
         <v>25</v>
       </c>
       <c r="J41" s="9"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
+      <c r="K41" s="18"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
       <c r="P41" s="9" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="Q41" s="7">
         <v>0</v>
@@ -1928,14 +2026,14 @@
     </row>
     <row r="42" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
+        <v>66</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
+      <c r="H42" s="18"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9" t="s">
         <v>25</v>
@@ -1946,11 +2044,11 @@
       <c r="L42" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
       <c r="P42" s="9" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="Q42" s="7">
         <v>0</v>
@@ -1958,14 +2056,14 @@
     </row>
     <row r="43" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C43" s="19"/>
-      <c r="D43" s="19"/>
-      <c r="E43" s="19"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
+        <v>68</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
+      <c r="G43" s="18"/>
+      <c r="H43" s="18"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="s">
         <v>25</v>
@@ -1976,11 +2074,11 @@
       <c r="L43" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M43" s="19"/>
-      <c r="N43" s="19"/>
-      <c r="O43" s="19"/>
+      <c r="M43" s="18"/>
+      <c r="N43" s="18"/>
+      <c r="O43" s="18"/>
       <c r="P43" s="9" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="Q43" s="7">
         <v>0</v>
@@ -1988,14 +2086,14 @@
     </row>
     <row r="44" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="19"/>
-      <c r="D44" s="19"/>
-      <c r="E44" s="19"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="19"/>
-      <c r="H44" s="19"/>
+        <v>70</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+      <c r="H44" s="18"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
         <v>25</v>
@@ -2006,57 +2104,55 @@
       <c r="L44" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19"/>
-      <c r="O44" s="19"/>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
       <c r="P44" s="9" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="Q44" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="21"/>
+      <c r="B45" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="20"/>
       <c r="J45" s="9"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
       <c r="P45" s="9"/>
-      <c r="Q45" s="7">
-        <v>0</v>
-      </c>
+      <c r="Q45" s="7"/>
     </row>
     <row r="46" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
+        <v>62</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
-      <c r="M46" s="19"/>
-      <c r="N46" s="19"/>
-      <c r="O46" s="19"/>
+      <c r="M46" s="18"/>
+      <c r="N46" s="18"/>
+      <c r="O46" s="18"/>
       <c r="P46" s="9" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="Q46" s="7">
         <v>1</v>
@@ -2064,7 +2160,7 @@
     </row>
     <row r="47" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="10" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2076,11 +2172,11 @@
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
-      <c r="M47" s="19"/>
-      <c r="N47" s="19"/>
-      <c r="O47" s="19"/>
+      <c r="M47" s="18"/>
+      <c r="N47" s="18"/>
+      <c r="O47" s="18"/>
       <c r="P47" s="9" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="Q47" s="7">
         <v>1</v>
@@ -2088,13 +2184,13 @@
     </row>
     <row r="48" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
+        <v>66</v>
+      </c>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9" t="s">
@@ -2107,10 +2203,10 @@
         <v>25</v>
       </c>
       <c r="M48" s="9"/>
-      <c r="N48" s="19"/>
-      <c r="O48" s="19"/>
+      <c r="N48" s="18"/>
+      <c r="O48" s="18"/>
       <c r="P48" s="9" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="Q48" s="7">
         <v>0</v>
@@ -2118,14 +2214,14 @@
     </row>
     <row r="49" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="19"/>
-      <c r="D49" s="19"/>
-      <c r="E49" s="19"/>
-      <c r="F49" s="19"/>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
+        <v>68</v>
+      </c>
+      <c r="C49" s="18"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="18"/>
+      <c r="G49" s="18"/>
+      <c r="H49" s="18"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9" t="s">
         <v>25</v>
@@ -2137,110 +2233,106 @@
         <v>25</v>
       </c>
       <c r="M49" s="9"/>
-      <c r="N49" s="19"/>
-      <c r="O49" s="19"/>
+      <c r="N49" s="18"/>
+      <c r="O49" s="18"/>
       <c r="P49" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q49" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K50" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="L50" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="M50" s="9"/>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q50" s="7">
+      <c r="B50" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="39"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="39"/>
+      <c r="I50" s="39"/>
+      <c r="J50" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="K50" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="L50" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
+      <c r="O50" s="39"/>
+      <c r="P50" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q50" s="41">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C51" s="19"/>
-      <c r="D51" s="19"/>
-      <c r="E51" s="19"/>
-      <c r="F51" s="19"/>
-      <c r="G51" s="19"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="12"/>
-      <c r="L51" s="12"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
-      <c r="O51" s="6"/>
-      <c r="P51" s="10"/>
-      <c r="Q51" s="7">
-        <v>0</v>
-      </c>
+      <c r="B51" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="49"/>
+      <c r="I51" s="49"/>
+      <c r="J51" s="49"/>
+      <c r="K51" s="49"/>
+      <c r="L51" s="49"/>
+      <c r="M51" s="49"/>
+      <c r="N51" s="49"/>
+      <c r="O51" s="49"/>
+      <c r="P51" s="49"/>
+      <c r="Q51" s="49"/>
     </row>
     <row r="52" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="19"/>
-      <c r="L52" s="19"/>
-      <c r="M52" s="19"/>
-      <c r="N52" s="19"/>
-      <c r="O52" s="19"/>
-      <c r="P52" s="25"/>
-      <c r="Q52" s="7">
-        <v>0</v>
-      </c>
+      <c r="B52" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="20"/>
+      <c r="L52" s="20"/>
+      <c r="M52" s="20"/>
+      <c r="N52" s="20"/>
+      <c r="O52" s="20"/>
+      <c r="P52" s="22"/>
+      <c r="Q52" s="29"/>
     </row>
     <row r="53" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="19"/>
-      <c r="D53" s="19"/>
-      <c r="E53" s="19"/>
-      <c r="F53" s="19"/>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
-      <c r="I53" s="19"/>
+        <v>75</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="18"/>
+      <c r="F53" s="18"/>
+      <c r="G53" s="18"/>
+      <c r="H53" s="18"/>
+      <c r="I53" s="18"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="N53" s="19"/>
-      <c r="O53" s="19"/>
+      <c r="N53" s="18"/>
+      <c r="O53" s="18"/>
       <c r="P53" s="9" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="Q53" s="7">
         <v>0</v>
@@ -2248,16 +2340,16 @@
     </row>
     <row r="54" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C54" s="19"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="19"/>
-      <c r="F54" s="19"/>
-      <c r="G54" s="19"/>
-      <c r="H54" s="21"/>
+        <v>76</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="18"/>
+      <c r="F54" s="18"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="20"/>
       <c r="I54" s="9"/>
-      <c r="J54" s="21"/>
+      <c r="J54" s="20"/>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9" t="s">
@@ -2266,9 +2358,9 @@
       <c r="N54" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O54" s="19"/>
+      <c r="O54" s="18"/>
       <c r="P54" s="9" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="Q54" s="7">
         <v>0</v>
@@ -2276,15 +2368,15 @@
     </row>
     <row r="55" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C55" s="19"/>
-      <c r="D55" s="19"/>
-      <c r="E55" s="19"/>
-      <c r="F55" s="19"/>
-      <c r="G55" s="19"/>
+        <v>78</v>
+      </c>
+      <c r="C55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="18"/>
+      <c r="F55" s="18"/>
+      <c r="G55" s="18"/>
       <c r="H55" s="9"/>
-      <c r="I55" s="19"/>
+      <c r="I55" s="18"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
@@ -2294,9 +2386,9 @@
       <c r="N55" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O55" s="19"/>
+      <c r="O55" s="18"/>
       <c r="P55" s="9" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="Q55" s="7">
         <v>0</v>
@@ -2304,15 +2396,15 @@
     </row>
     <row r="56" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="19"/>
-      <c r="G56" s="19"/>
-      <c r="H56" s="19"/>
-      <c r="I56" s="19"/>
+        <v>80</v>
+      </c>
+      <c r="C56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="18"/>
+      <c r="H56" s="18"/>
+      <c r="I56" s="18"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
@@ -2322,9 +2414,9 @@
       <c r="N56" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O56" s="19"/>
-      <c r="P56" s="25" t="s">
-        <v>95</v>
+      <c r="O56" s="18"/>
+      <c r="P56" s="22" t="s">
+        <v>81</v>
       </c>
       <c r="Q56" s="7">
         <v>0</v>
@@ -2332,14 +2424,14 @@
     </row>
     <row r="57" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C57" s="19"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="19"/>
-      <c r="H57" s="19"/>
+        <v>82</v>
+      </c>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
@@ -2350,9 +2442,9 @@
       <c r="N57" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O57" s="19"/>
+      <c r="O57" s="18"/>
       <c r="P57" s="10" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="Q57" s="7">
         <v>0</v>
@@ -2360,15 +2452,15 @@
     </row>
     <row r="58" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="C58" s="19"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="19"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
+        <v>84</v>
+      </c>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+      <c r="E58" s="18"/>
+      <c r="F58" s="18"/>
+      <c r="G58" s="18"/>
+      <c r="H58" s="18"/>
+      <c r="I58" s="18"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
@@ -2380,55 +2472,53 @@
       </c>
       <c r="O58" s="9"/>
       <c r="P58" s="10" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="Q58" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
+      <c r="B59" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="18"/>
+      <c r="G59" s="18"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="18"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
-      <c r="M59" s="19"/>
+      <c r="M59" s="18"/>
       <c r="N59" s="9"/>
       <c r="O59" s="9"/>
-      <c r="P59" s="25"/>
-      <c r="Q59" s="7">
-        <v>0</v>
-      </c>
+      <c r="P59" s="22"/>
+      <c r="Q59" s="7"/>
     </row>
     <row r="60" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
+        <v>86</v>
+      </c>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
       <c r="M60" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="N60" s="12"/>
+      <c r="N60" s="11"/>
       <c r="O60" s="9"/>
       <c r="P60" s="9" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="Q60" s="7">
         <v>0</v>
@@ -2436,25 +2526,25 @@
     </row>
     <row r="61" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C61" s="19"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="19"/>
-      <c r="F61" s="19"/>
-      <c r="G61" s="19"/>
-      <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
+        <v>75</v>
+      </c>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="18"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="18"/>
+      <c r="L61" s="18"/>
       <c r="M61" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="N61" s="12"/>
+      <c r="N61" s="11"/>
       <c r="O61" s="9"/>
-      <c r="P61" s="26" t="s">
-        <v>101</v>
+      <c r="P61" s="23" t="s">
+        <v>87</v>
       </c>
       <c r="Q61" s="7">
         <v>0</v>
@@ -2462,27 +2552,27 @@
     </row>
     <row r="62" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C62" s="19"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="19"/>
-      <c r="G62" s="19"/>
-      <c r="H62" s="21"/>
+        <v>76</v>
+      </c>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+      <c r="H62" s="20"/>
       <c r="I62" s="9"/>
-      <c r="J62" s="21"/>
+      <c r="J62" s="20"/>
       <c r="K62" s="9"/>
-      <c r="L62" s="19"/>
+      <c r="L62" s="18"/>
       <c r="M62" s="9" t="s">
         <v>25</v>
       </c>
       <c r="N62" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O62" s="19"/>
+      <c r="O62" s="18"/>
       <c r="P62" s="9" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="Q62" s="7">
         <v>0</v>
@@ -2490,27 +2580,27 @@
     </row>
     <row r="63" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
+        <v>78</v>
+      </c>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
       <c r="H63" s="9"/>
-      <c r="I63" s="19"/>
+      <c r="I63" s="18"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
-      <c r="L63" s="19"/>
+      <c r="L63" s="18"/>
       <c r="M63" s="9" t="s">
         <v>25</v>
       </c>
       <c r="N63" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O63" s="19"/>
+      <c r="O63" s="18"/>
       <c r="P63" s="9" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="Q63" s="7">
         <v>0</v>
@@ -2518,18 +2608,18 @@
     </row>
     <row r="64" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="19"/>
-      <c r="F64" s="19"/>
-      <c r="G64" s="19"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
-      <c r="J64" s="19"/>
-      <c r="K64" s="19"/>
-      <c r="L64" s="19"/>
+        <v>80</v>
+      </c>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18"/>
+      <c r="G64" s="18"/>
+      <c r="H64" s="18"/>
+      <c r="I64" s="18"/>
+      <c r="J64" s="18"/>
+      <c r="K64" s="18"/>
+      <c r="L64" s="18"/>
       <c r="M64" s="9" t="s">
         <v>25</v>
       </c>
@@ -2537,8 +2627,8 @@
         <v>25</v>
       </c>
       <c r="O64" s="9"/>
-      <c r="P64" s="26" t="s">
-        <v>87</v>
+      <c r="P64" s="23" t="s">
+        <v>73</v>
       </c>
       <c r="Q64" s="7">
         <v>0</v>
@@ -2546,18 +2636,18 @@
     </row>
     <row r="65" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="19"/>
-      <c r="F65" s="19"/>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
-      <c r="J65" s="19"/>
-      <c r="K65" s="19"/>
-      <c r="L65" s="19"/>
+        <v>82</v>
+      </c>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="18"/>
+      <c r="F65" s="18"/>
+      <c r="G65" s="18"/>
+      <c r="H65" s="18"/>
+      <c r="I65" s="18"/>
+      <c r="J65" s="18"/>
+      <c r="K65" s="18"/>
+      <c r="L65" s="18"/>
       <c r="M65" s="9" t="s">
         <v>25</v>
       </c>
@@ -2565,27 +2655,27 @@
         <v>25</v>
       </c>
       <c r="O65" s="9"/>
-      <c r="P65" s="26" t="s">
-        <v>103</v>
+      <c r="P65" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="Q65" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C66" s="28"/>
-      <c r="D66" s="28"/>
-      <c r="E66" s="28"/>
-      <c r="F66" s="28"/>
-      <c r="G66" s="28"/>
-      <c r="H66" s="28"/>
-      <c r="I66" s="19"/>
-      <c r="J66" s="19"/>
-      <c r="K66" s="19"/>
-      <c r="L66" s="19"/>
+      <c r="B66" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="18"/>
+      <c r="J66" s="18"/>
+      <c r="K66" s="18"/>
+      <c r="L66" s="18"/>
       <c r="M66" s="9" t="s">
         <v>25</v>
       </c>
@@ -2594,26 +2684,26 @@
       </c>
       <c r="O66" s="9"/>
       <c r="P66" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q66" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="28"/>
-      <c r="F67" s="28"/>
-      <c r="G67" s="28"/>
-      <c r="H67" s="28"/>
-      <c r="I67" s="19"/>
-      <c r="J67" s="19"/>
-      <c r="K67" s="19"/>
-      <c r="L67" s="19"/>
+      <c r="B67" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="18"/>
+      <c r="J67" s="18"/>
+      <c r="K67" s="18"/>
+      <c r="L67" s="18"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
       <c r="O67" s="9"/>
@@ -2624,18 +2714,18 @@
     </row>
     <row r="68" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="28"/>
-      <c r="F68" s="28"/>
-      <c r="G68" s="28"/>
-      <c r="H68" s="28"/>
-      <c r="I68" s="19"/>
-      <c r="J68" s="19"/>
-      <c r="K68" s="19"/>
-      <c r="L68" s="19"/>
+        <v>91</v>
+      </c>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="18"/>
+      <c r="J68" s="18"/>
+      <c r="K68" s="18"/>
+      <c r="L68" s="18"/>
       <c r="M68" s="9"/>
       <c r="N68" s="9" t="s">
         <v>25</v>
@@ -2644,7 +2734,7 @@
         <v>25</v>
       </c>
       <c r="P68" s="9" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="Q68" s="7">
         <v>0</v>
@@ -2652,18 +2742,18 @@
     </row>
     <row r="69" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="28"/>
-      <c r="F69" s="28"/>
-      <c r="G69" s="28"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="19"/>
-      <c r="J69" s="19"/>
-      <c r="K69" s="19"/>
-      <c r="L69" s="19"/>
+        <v>93</v>
+      </c>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
+      <c r="L69" s="18"/>
       <c r="M69" s="9"/>
       <c r="N69" s="9" t="s">
         <v>25</v>
@@ -2672,187 +2762,187 @@
         <v>25</v>
       </c>
       <c r="P69" s="9" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="Q69" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C70" s="28"/>
-      <c r="D70" s="28"/>
-      <c r="E70" s="28"/>
-      <c r="F70" s="28"/>
-      <c r="G70" s="28"/>
-      <c r="H70" s="28"/>
-      <c r="I70" s="19"/>
-      <c r="J70" s="19"/>
-      <c r="K70" s="19"/>
-      <c r="L70" s="19"/>
-      <c r="M70" s="9"/>
-      <c r="N70" s="12"/>
-      <c r="O70" s="12"/>
-      <c r="P70" s="12"/>
-      <c r="Q70" s="7">
+      <c r="B70" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="18"/>
+      <c r="J70" s="18"/>
+      <c r="K70" s="18"/>
+      <c r="L70" s="18"/>
+      <c r="M70" s="18"/>
+      <c r="N70" s="18"/>
+      <c r="O70" s="18"/>
+      <c r="P70" s="18"/>
+      <c r="Q70" s="26">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C71" s="28"/>
-      <c r="D71" s="28"/>
-      <c r="E71" s="28"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="28"/>
-      <c r="H71" s="28"/>
-      <c r="I71" s="19"/>
-      <c r="J71" s="19"/>
-      <c r="K71" s="19"/>
-      <c r="L71" s="9"/>
-      <c r="M71" s="19"/>
-      <c r="N71" s="12"/>
-      <c r="O71" s="12"/>
-      <c r="P71" s="12"/>
-      <c r="Q71" s="31">
+      <c r="B71" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="24"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="24"/>
+      <c r="J71" s="24"/>
+      <c r="K71" s="24"/>
+      <c r="L71" s="27"/>
+      <c r="M71" s="28"/>
+      <c r="N71" s="18"/>
+      <c r="O71" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="P71" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q71" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="72" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C72" s="28"/>
-      <c r="D72" s="28"/>
-      <c r="E72" s="28"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="28"/>
-      <c r="H72" s="28"/>
-      <c r="I72" s="28"/>
-      <c r="J72" s="28"/>
-      <c r="K72" s="28"/>
-      <c r="L72" s="32"/>
-      <c r="M72" s="33"/>
-      <c r="N72" s="12"/>
-      <c r="O72" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P72" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q72" s="34">
+      <c r="B72" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" s="24"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="24"/>
+      <c r="J72" s="24"/>
+      <c r="K72" s="24"/>
+      <c r="L72" s="24"/>
+      <c r="M72" s="24"/>
+      <c r="N72" s="18"/>
+      <c r="O72" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="P72" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q72" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
-      <c r="E73" s="28"/>
-      <c r="F73" s="28"/>
-      <c r="G73" s="28"/>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="28"/>
-      <c r="K73" s="28"/>
-      <c r="L73" s="28"/>
-      <c r="M73" s="28"/>
-      <c r="N73" s="19"/>
-      <c r="O73" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P73" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q73" s="34">
+      <c r="B73" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="24"/>
+      <c r="J73" s="24"/>
+      <c r="K73" s="24"/>
+      <c r="L73" s="24"/>
+      <c r="M73" s="24"/>
+      <c r="N73" s="18"/>
+      <c r="O73" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="P73" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q73" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C74" s="28"/>
-      <c r="D74" s="28"/>
-      <c r="E74" s="28"/>
-      <c r="F74" s="28"/>
-      <c r="G74" s="28"/>
-      <c r="H74" s="28"/>
-      <c r="I74" s="28"/>
-      <c r="J74" s="28"/>
-      <c r="K74" s="28"/>
-      <c r="L74" s="28"/>
-      <c r="M74" s="28"/>
-      <c r="N74" s="19"/>
-      <c r="O74" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P74" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q74" s="34">
+      <c r="B74" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="24"/>
+      <c r="J74" s="24"/>
+      <c r="K74" s="24"/>
+      <c r="L74" s="24"/>
+      <c r="M74" s="24"/>
+      <c r="N74" s="18"/>
+      <c r="O74" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="P74" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q74" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C75" s="28"/>
-      <c r="D75" s="28"/>
-      <c r="E75" s="28"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="28"/>
-      <c r="H75" s="28"/>
-      <c r="I75" s="28"/>
-      <c r="J75" s="28"/>
-      <c r="K75" s="28"/>
-      <c r="L75" s="28"/>
-      <c r="M75" s="28"/>
-      <c r="N75" s="19"/>
-      <c r="O75" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P75" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q75" s="34">
+      <c r="B75" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="43"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="43"/>
+      <c r="I75" s="43"/>
+      <c r="J75" s="43"/>
+      <c r="K75" s="43"/>
+      <c r="L75" s="43"/>
+      <c r="M75" s="43"/>
+      <c r="N75" s="39"/>
+      <c r="O75" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="P75" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q75" s="46">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="C76" s="28"/>
-      <c r="D76" s="28"/>
-      <c r="E76" s="28"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="28"/>
-      <c r="H76" s="28"/>
-      <c r="I76" s="28"/>
-      <c r="J76" s="28"/>
-      <c r="K76" s="28"/>
-      <c r="L76" s="28"/>
-      <c r="M76" s="28"/>
-      <c r="N76" s="19"/>
-      <c r="O76" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="P76" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q76" s="34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B76" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="47"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="47"/>
+      <c r="H76" s="47"/>
+      <c r="I76" s="47"/>
+      <c r="J76" s="47"/>
+      <c r="K76" s="47"/>
+      <c r="L76" s="47"/>
+      <c r="M76" s="47"/>
+      <c r="N76" s="47"/>
+      <c r="O76" s="47"/>
+      <c r="P76" s="47"/>
+      <c r="Q76" s="47"/>
+    </row>
+    <row r="77" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="38"/>
+    </row>
     <row r="78" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3749,7 +3839,10 @@
     <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="B33:Q33"/>
+    <mergeCell ref="B51:Q51"/>
+    <mergeCell ref="B76:Q76"/>
     <mergeCell ref="B11:Q11"/>
     <mergeCell ref="B1:Q1"/>
     <mergeCell ref="C2:Q2"/>

</xml_diff>

<commit_message>
Se actualizo el cronograma
</commit_message>
<xml_diff>
--- a/Desarrollo/SHS/Gestión/SHS-CP.xlsx
+++ b/Desarrollo/SHS/Gestión/SHS-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Jose Tirado\OneDrive\Escritorio\6to ciclo\ProyectoGestionConfig\ServiceHomeStore\Desarrollo\SHS\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A9B859-0B05-40A4-90E8-C26346D6862A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E8F23F-F0C8-4941-8838-53BE1AA1EB6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yy"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,6 +518,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -653,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -699,6 +706,34 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -715,33 +750,6 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -959,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH972"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -975,46 +983,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:34" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
     </row>
     <row r="2" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
@@ -1034,67 +1042,67 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
+      <c r="L3" s="52"/>
+      <c r="M3" s="52"/>
+      <c r="N3" s="52"/>
+      <c r="O3" s="52"/>
+      <c r="P3" s="52"/>
+      <c r="Q3" s="52"/>
     </row>
     <row r="4" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="35">
+      <c r="C4" s="55">
         <v>44132</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
     </row>
     <row r="5" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="56">
         <v>44216</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
     </row>
     <row r="6" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -1229,57 +1237,57 @@
       </c>
     </row>
     <row r="10" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="52" t="s">
+      <c r="B10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39" t="s">
+      <c r="C10" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="Q10" s="41">
+      <c r="Q10" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="53" t="s">
+      <c r="B11" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="54"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="54"/>
-      <c r="P11" s="54"/>
-      <c r="Q11" s="54"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="50"/>
+      <c r="N11" s="50"/>
+      <c r="O11" s="50"/>
+      <c r="P11" s="50"/>
+      <c r="Q11" s="50"/>
     </row>
     <row r="12" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="50" t="s">
+      <c r="B12" s="42" t="s">
         <v>32</v>
       </c>
       <c r="C12" s="20"/>
@@ -1789,53 +1797,53 @@
       </c>
     </row>
     <row r="32" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="39" t="s">
+      <c r="B32" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="I32" s="40"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39"/>
-      <c r="P32" s="39" t="s">
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="34"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="Q32" s="41">
+      <c r="Q32" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="51" t="s">
+    <row r="33" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="51"/>
-      <c r="I33" s="51"/>
-      <c r="J33" s="51"/>
-      <c r="K33" s="51"/>
-      <c r="L33" s="51"/>
-      <c r="M33" s="51"/>
-      <c r="N33" s="51"/>
-      <c r="O33" s="51"/>
-      <c r="P33" s="51"/>
-      <c r="Q33" s="51"/>
-    </row>
-    <row r="34" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="50" t="s">
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+    </row>
+    <row r="34" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="42" t="s">
         <v>58</v>
       </c>
       <c r="C34" s="20"/>
@@ -1854,7 +1862,7 @@
       <c r="P34" s="20"/>
       <c r="Q34" s="29"/>
     </row>
-    <row r="35" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
         <v>59</v>
       </c>
@@ -1880,7 +1888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
         <v>60</v>
       </c>
@@ -1906,8 +1914,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="55" t="s">
+    <row r="37" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="44" t="s">
         <v>123</v>
       </c>
       <c r="C37" s="18"/>
@@ -1926,7 +1934,7 @@
       <c r="P37" s="9"/>
       <c r="Q37" s="7"/>
     </row>
-    <row r="38" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="21" t="s">
         <v>61</v>
       </c>
@@ -1945,8 +1953,9 @@
       <c r="O38" s="18"/>
       <c r="P38" s="9"/>
       <c r="Q38" s="7"/>
-    </row>
-    <row r="39" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R38" s="45"/>
+    </row>
+    <row r="39" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
         <v>62</v>
       </c>
@@ -1972,7 +1981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>63</v>
       </c>
@@ -1998,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
         <v>65</v>
       </c>
@@ -2021,10 +2030,10 @@
         <v>50</v>
       </c>
       <c r="Q41" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10" t="s">
         <v>66</v>
       </c>
@@ -2054,7 +2063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="10" t="s">
         <v>68</v>
       </c>
@@ -2084,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
         <v>70</v>
       </c>
@@ -2114,7 +2123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="21" t="s">
         <v>71</v>
       </c>
@@ -2134,7 +2143,7 @@
       <c r="P45" s="9"/>
       <c r="Q45" s="7"/>
     </row>
-    <row r="46" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
         <v>62</v>
       </c>
@@ -2158,7 +2167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="10" t="s">
         <v>63</v>
       </c>
@@ -2182,7 +2191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
         <v>66</v>
       </c>
@@ -2209,7 +2218,7 @@
         <v>73</v>
       </c>
       <c r="Q48" s="7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="49" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2239,61 +2248,61 @@
         <v>39</v>
       </c>
       <c r="Q49" s="7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="50" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="39" t="s">
+      <c r="B50" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="39"/>
-      <c r="D50" s="39"/>
-      <c r="E50" s="39"/>
-      <c r="F50" s="39"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="39"/>
-      <c r="I50" s="39"/>
-      <c r="J50" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="K50" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="L50" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="M50" s="39"/>
-      <c r="N50" s="39"/>
-      <c r="O50" s="39"/>
-      <c r="P50" s="39" t="s">
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
+      <c r="J50" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="K50" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="L50" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="33"/>
+      <c r="N50" s="33"/>
+      <c r="O50" s="33"/>
+      <c r="P50" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="Q50" s="41">
-        <v>0</v>
+      <c r="Q50" s="35">
+        <v>0.1</v>
       </c>
     </row>
     <row r="51" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="49" t="s">
+      <c r="B51" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="49"/>
-      <c r="H51" s="49"/>
-      <c r="I51" s="49"/>
-      <c r="J51" s="49"/>
-      <c r="K51" s="49"/>
-      <c r="L51" s="49"/>
-      <c r="M51" s="49"/>
-      <c r="N51" s="49"/>
-      <c r="O51" s="49"/>
-      <c r="P51" s="49"/>
-      <c r="Q51" s="49"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="47"/>
+      <c r="H51" s="47"/>
+      <c r="I51" s="47"/>
+      <c r="J51" s="47"/>
+      <c r="K51" s="47"/>
+      <c r="L51" s="47"/>
+      <c r="M51" s="47"/>
+      <c r="N51" s="47"/>
+      <c r="O51" s="47"/>
+      <c r="P51" s="47"/>
+      <c r="Q51" s="47"/>
     </row>
     <row r="52" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="48" t="s">
+      <c r="B52" s="41" t="s">
         <v>61</v>
       </c>
       <c r="C52" s="20"/>
@@ -2663,7 +2672,7 @@
       </c>
     </row>
     <row r="66" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="37" t="s">
+      <c r="B66" s="31" t="s">
         <v>84</v>
       </c>
       <c r="C66" s="24"/>
@@ -2887,7 +2896,7 @@
       <c r="O74" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="P74" s="39" t="s">
+      <c r="P74" s="33" t="s">
         <v>99</v>
       </c>
       <c r="Q74" s="29">
@@ -2895,53 +2904,53 @@
       </c>
     </row>
     <row r="75" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="42" t="s">
+      <c r="B75" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="43"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="43"/>
-      <c r="I75" s="43"/>
-      <c r="J75" s="43"/>
-      <c r="K75" s="43"/>
-      <c r="L75" s="43"/>
-      <c r="M75" s="43"/>
-      <c r="N75" s="39"/>
-      <c r="O75" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="P75" s="45" t="s">
+      <c r="C75" s="37"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="37"/>
+      <c r="G75" s="37"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
+      <c r="J75" s="37"/>
+      <c r="K75" s="37"/>
+      <c r="L75" s="37"/>
+      <c r="M75" s="37"/>
+      <c r="N75" s="33"/>
+      <c r="O75" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="P75" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="Q75" s="46">
+      <c r="Q75" s="40">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="47" t="s">
+      <c r="B76" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="C76" s="47"/>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
-      <c r="H76" s="47"/>
-      <c r="I76" s="47"/>
-      <c r="J76" s="47"/>
-      <c r="K76" s="47"/>
-      <c r="L76" s="47"/>
-      <c r="M76" s="47"/>
-      <c r="N76" s="47"/>
-      <c r="O76" s="47"/>
-      <c r="P76" s="47"/>
-      <c r="Q76" s="47"/>
+      <c r="C76" s="48"/>
+      <c r="D76" s="48"/>
+      <c r="E76" s="48"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="48"/>
+      <c r="H76" s="48"/>
+      <c r="I76" s="48"/>
+      <c r="J76" s="48"/>
+      <c r="K76" s="48"/>
+      <c r="L76" s="48"/>
+      <c r="M76" s="48"/>
+      <c r="N76" s="48"/>
+      <c r="O76" s="48"/>
+      <c r="P76" s="48"/>
+      <c r="Q76" s="48"/>
     </row>
     <row r="77" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="38"/>
+      <c r="B77" s="32"/>
     </row>
     <row r="78" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se avanzo con la codificacion para agregar servicios
</commit_message>
<xml_diff>
--- a/Desarrollo/SHS/Gestión/SHS-CP.xlsx
+++ b/Desarrollo/SHS/Gestión/SHS-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Jose Tirado\OneDrive\Escritorio\6to ciclo\ProyectoGestionConfig\ServiceHomeStore\Desarrollo\SHS\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E8F23F-F0C8-4941-8838-53BE1AA1EB6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0A5EDA-BD7A-45CB-A867-1664C50805D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1172,9 +1172,7 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
-      <c r="Q7" s="7">
-        <v>1</v>
-      </c>
+      <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
@@ -2060,7 +2058,7 @@
         <v>67</v>
       </c>
       <c r="Q42" s="7">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="43" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2218,7 +2216,7 @@
         <v>73</v>
       </c>
       <c r="Q48" s="7">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="49" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2248,7 +2246,7 @@
         <v>39</v>
       </c>
       <c r="Q49" s="7">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="50" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2278,7 +2276,7 @@
         <v>39</v>
       </c>
       <c r="Q50" s="35">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Se agrego carpetas de los clientes y se actualizo el CP
</commit_message>
<xml_diff>
--- a/Desarrollo/SHS/Gestión/SHS-CP.xlsx
+++ b/Desarrollo/SHS/Gestión/SHS-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Jose Tirado\OneDrive\Escritorio\6to ciclo\ProyectoGestionConfig\ServiceHomeStore\Desarrollo\SHS\Gestión\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Jose Tirado\OneDrive\Escritorio\6to ciclo\PROYECTO FINAL GC\ServiceHomeStore\Desarrollo\SHS\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD72C02-E693-4F13-9586-52350E7C8D36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF65CCF-66C6-411E-8F03-B54DB72D3793}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R61" sqref="R61"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S65" sqref="S65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2342,7 @@
         <v>64</v>
       </c>
       <c r="Q53" s="7">
-        <v>0.15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2370,7 +2370,7 @@
         <v>77</v>
       </c>
       <c r="Q54" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2398,7 +2398,7 @@
         <v>79</v>
       </c>
       <c r="Q55" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2426,7 +2426,7 @@
         <v>81</v>
       </c>
       <c r="Q56" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2454,7 +2454,7 @@
         <v>83</v>
       </c>
       <c r="Q57" s="7">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="58" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2482,7 +2482,7 @@
         <v>85</v>
       </c>
       <c r="Q58" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2528,7 +2528,7 @@
         <v>85</v>
       </c>
       <c r="Q60" s="7">
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2554,7 +2554,7 @@
         <v>87</v>
       </c>
       <c r="Q61" s="7">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="R61" s="45"/>
     </row>
@@ -2583,7 +2583,7 @@
         <v>73</v>
       </c>
       <c r="Q62" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2611,7 +2611,7 @@
         <v>88</v>
       </c>
       <c r="Q63" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2639,10 +2639,10 @@
         <v>73</v>
       </c>
       <c r="Q64" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="10" t="s">
         <v>82</v>
       </c>
@@ -2667,10 +2667,11 @@
         <v>89</v>
       </c>
       <c r="Q65" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+      <c r="S65" s="45"/>
+    </row>
+    <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="31" t="s">
         <v>84</v>
       </c>
@@ -2695,10 +2696,10 @@
         <v>39</v>
       </c>
       <c r="Q66" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="17" t="s">
         <v>90</v>
       </c>
@@ -2720,7 +2721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="10" t="s">
         <v>91</v>
       </c>
@@ -2748,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="10" t="s">
         <v>93</v>
       </c>
@@ -2776,7 +2777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="25" t="s">
         <v>95</v>
       </c>
@@ -2798,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="18" t="s">
         <v>96</v>
       </c>
@@ -2824,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="18" t="s">
         <v>98</v>
       </c>
@@ -2850,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="18" t="s">
         <v>100</v>
       </c>
@@ -2876,7 +2877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="18" t="s">
         <v>102</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="36" t="s">
         <v>103</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="48" t="s">
         <v>122</v>
       </c>
@@ -2948,12 +2949,12 @@
       <c r="P76" s="48"/>
       <c r="Q76" s="48"/>
     </row>
-    <row r="77" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="32"/>
     </row>
-    <row r="78" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se actualizo las tablas de la base de datos
</commit_message>
<xml_diff>
--- a/Desarrollo/SHS/Gestión/SHS-CP.xlsx
+++ b/Desarrollo/SHS/Gestión/SHS-CP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Jose Tirado\OneDrive\Escritorio\6to ciclo\PROYECTO FINAL GC\ServiceHomeStore\Desarrollo\SHS\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF65CCF-66C6-411E-8F03-B54DB72D3793}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8963E9CA-8080-450B-A131-A5756F1C558E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -123,9 +123,6 @@
     <t>Hito #1: 11/11/2020</t>
   </si>
   <si>
-    <t>Elaboracion decumento de especificación de requisitos</t>
-  </si>
-  <si>
     <t>Elaboración de la especificación del requisito 01: Login</t>
   </si>
   <si>
@@ -397,6 +394,9 @@
   </si>
   <si>
     <t>Codificacion</t>
+  </si>
+  <si>
+    <t>Elaboracion documento de especificación de requisitos</t>
   </si>
 </sst>
 </file>
@@ -660,7 +660,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -750,6 +750,7 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -967,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S65" sqref="S65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1285,8 +1286,8 @@
       <c r="Q11" s="50"/>
     </row>
     <row r="12" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="42" t="s">
-        <v>32</v>
+      <c r="B12" s="57" t="s">
+        <v>123</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -1306,7 +1307,7 @@
     </row>
     <row r="13" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B13" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1324,7 +1325,7 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q13" s="7">
         <v>1</v>
@@ -1332,7 +1333,7 @@
     </row>
     <row r="14" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -1350,7 +1351,7 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q14" s="7">
         <v>1</v>
@@ -1358,7 +1359,7 @@
     </row>
     <row r="15" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -1378,7 +1379,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q15" s="7">
         <v>1</v>
@@ -1386,7 +1387,7 @@
     </row>
     <row r="16" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B16" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -1406,7 +1407,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q16" s="7">
         <v>1</v>
@@ -1414,7 +1415,7 @@
     </row>
     <row r="17" spans="2:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B17" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -1434,7 +1435,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q17" s="15">
         <v>1</v>
@@ -1442,7 +1443,7 @@
     </row>
     <row r="18" spans="2:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B18" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -1462,7 +1463,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q18" s="7">
         <v>1</v>
@@ -1470,7 +1471,7 @@
     </row>
     <row r="19" spans="2:17" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B19" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -1488,7 +1489,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q19" s="7">
         <v>1</v>
@@ -1496,7 +1497,7 @@
     </row>
     <row r="20" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
@@ -1514,7 +1515,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q20" s="7">
         <v>1</v>
@@ -1522,7 +1523,7 @@
     </row>
     <row r="21" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -1540,7 +1541,7 @@
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q21" s="7">
         <v>1</v>
@@ -1548,7 +1549,7 @@
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1566,7 +1567,7 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q22" s="7">
         <v>1</v>
@@ -1574,7 +1575,7 @@
     </row>
     <row r="23" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1592,7 +1593,7 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q23" s="7">
         <v>1</v>
@@ -1600,7 +1601,7 @@
     </row>
     <row r="24" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1618,7 +1619,7 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q24" s="7">
         <v>1</v>
@@ -1626,7 +1627,7 @@
     </row>
     <row r="25" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1646,7 +1647,7 @@
     </row>
     <row r="26" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1664,7 +1665,7 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q26" s="7">
         <v>1</v>
@@ -1672,7 +1673,7 @@
     </row>
     <row r="27" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1690,7 +1691,7 @@
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q27" s="7">
         <v>1</v>
@@ -1698,7 +1699,7 @@
     </row>
     <row r="28" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="18"/>
@@ -1716,7 +1717,7 @@
       <c r="N28" s="18"/>
       <c r="O28" s="18"/>
       <c r="P28" s="30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q28" s="7">
         <v>1</v>
@@ -1724,7 +1725,7 @@
     </row>
     <row r="29" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
@@ -1744,7 +1745,7 @@
     </row>
     <row r="30" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="18"/>
@@ -1762,7 +1763,7 @@
       <c r="N30" s="18"/>
       <c r="O30" s="18"/>
       <c r="P30" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q30" s="7">
         <v>1</v>
@@ -1770,7 +1771,7 @@
     </row>
     <row r="31" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
@@ -1788,7 +1789,7 @@
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
       <c r="P31" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q31" s="7">
         <v>1</v>
@@ -1796,7 +1797,7 @@
     </row>
     <row r="32" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="33"/>
       <c r="D32" s="33"/>
@@ -1814,7 +1815,7 @@
       <c r="N32" s="33"/>
       <c r="O32" s="33"/>
       <c r="P32" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q32" s="35">
         <v>1</v>
@@ -1822,7 +1823,7 @@
     </row>
     <row r="33" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" s="46"/>
       <c r="D33" s="46"/>
@@ -1842,7 +1843,7 @@
     </row>
     <row r="34" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C34" s="20"/>
       <c r="D34" s="20"/>
@@ -1862,7 +1863,7 @@
     </row>
     <row r="35" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="18"/>
@@ -1880,7 +1881,7 @@
       <c r="N35" s="18"/>
       <c r="O35" s="18"/>
       <c r="P35" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q35" s="7">
         <v>1</v>
@@ -1888,7 +1889,7 @@
     </row>
     <row r="36" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="18"/>
@@ -1906,7 +1907,7 @@
       <c r="N36" s="18"/>
       <c r="O36" s="18"/>
       <c r="P36" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q36" s="7">
         <v>1</v>
@@ -1914,7 +1915,7 @@
     </row>
     <row r="37" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="44" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -1934,7 +1935,7 @@
     </row>
     <row r="38" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C38" s="18"/>
       <c r="D38" s="18"/>
@@ -1955,7 +1956,7 @@
     </row>
     <row r="39" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -1973,7 +1974,7 @@
       <c r="N39" s="18"/>
       <c r="O39" s="18"/>
       <c r="P39" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q39" s="7">
         <v>1</v>
@@ -1981,7 +1982,7 @@
     </row>
     <row r="40" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
@@ -1999,7 +2000,7 @@
       <c r="N40" s="18"/>
       <c r="O40" s="18"/>
       <c r="P40" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q40" s="7">
         <v>1</v>
@@ -2007,7 +2008,7 @@
     </row>
     <row r="41" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -2025,7 +2026,7 @@
       <c r="N41" s="18"/>
       <c r="O41" s="18"/>
       <c r="P41" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q41" s="7">
         <v>1</v>
@@ -2033,7 +2034,7 @@
     </row>
     <row r="42" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -2055,7 +2056,7 @@
       <c r="N42" s="18"/>
       <c r="O42" s="18"/>
       <c r="P42" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q42" s="7">
         <v>1</v>
@@ -2063,7 +2064,7 @@
     </row>
     <row r="43" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -2085,7 +2086,7 @@
       <c r="N43" s="18"/>
       <c r="O43" s="18"/>
       <c r="P43" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q43" s="7">
         <v>1</v>
@@ -2093,7 +2094,7 @@
     </row>
     <row r="44" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
@@ -2115,7 +2116,7 @@
       <c r="N44" s="18"/>
       <c r="O44" s="18"/>
       <c r="P44" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="Q44" s="7">
         <v>1</v>
@@ -2123,7 +2124,7 @@
     </row>
     <row r="45" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -2143,7 +2144,7 @@
     </row>
     <row r="46" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -2159,7 +2160,7 @@
       <c r="N46" s="18"/>
       <c r="O46" s="18"/>
       <c r="P46" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q46" s="7">
         <v>1</v>
@@ -2167,7 +2168,7 @@
     </row>
     <row r="47" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2183,7 +2184,7 @@
       <c r="N47" s="18"/>
       <c r="O47" s="18"/>
       <c r="P47" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q47" s="7">
         <v>1</v>
@@ -2191,7 +2192,7 @@
     </row>
     <row r="48" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
@@ -2213,7 +2214,7 @@
       <c r="N48" s="18"/>
       <c r="O48" s="18"/>
       <c r="P48" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q48" s="7">
         <v>1</v>
@@ -2221,7 +2222,7 @@
     </row>
     <row r="49" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
@@ -2243,7 +2244,7 @@
       <c r="N49" s="18"/>
       <c r="O49" s="18"/>
       <c r="P49" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q49" s="7">
         <v>1</v>
@@ -2251,7 +2252,7 @@
     </row>
     <row r="50" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
@@ -2273,7 +2274,7 @@
       <c r="N50" s="33"/>
       <c r="O50" s="33"/>
       <c r="P50" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q50" s="35">
         <v>1</v>
@@ -2281,7 +2282,7 @@
     </row>
     <row r="51" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="47" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="47"/>
       <c r="D51" s="47"/>
@@ -2301,7 +2302,7 @@
     </row>
     <row r="52" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C52" s="20"/>
       <c r="D52" s="20"/>
@@ -2321,7 +2322,7 @@
     </row>
     <row r="53" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
@@ -2339,7 +2340,7 @@
       <c r="N53" s="18"/>
       <c r="O53" s="18"/>
       <c r="P53" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q53" s="7">
         <v>1</v>
@@ -2347,7 +2348,7 @@
     </row>
     <row r="54" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
@@ -2367,7 +2368,7 @@
       </c>
       <c r="O54" s="18"/>
       <c r="P54" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q54" s="7">
         <v>1</v>
@@ -2375,7 +2376,7 @@
     </row>
     <row r="55" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -2395,7 +2396,7 @@
       </c>
       <c r="O55" s="18"/>
       <c r="P55" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q55" s="7">
         <v>1</v>
@@ -2403,7 +2404,7 @@
     </row>
     <row r="56" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
@@ -2423,7 +2424,7 @@
       </c>
       <c r="O56" s="18"/>
       <c r="P56" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="Q56" s="7">
         <v>1</v>
@@ -2431,7 +2432,7 @@
     </row>
     <row r="57" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
@@ -2451,15 +2452,15 @@
       </c>
       <c r="O57" s="18"/>
       <c r="P57" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Q57" s="7">
-        <v>0.6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
@@ -2479,7 +2480,7 @@
       </c>
       <c r="O58" s="9"/>
       <c r="P58" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q58" s="7">
         <v>1</v>
@@ -2487,7 +2488,7 @@
     </row>
     <row r="59" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="18"/>
@@ -2507,7 +2508,7 @@
     </row>
     <row r="60" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
@@ -2525,7 +2526,7 @@
       <c r="N60" s="11"/>
       <c r="O60" s="9"/>
       <c r="P60" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="Q60" s="7">
         <v>1</v>
@@ -2533,7 +2534,7 @@
     </row>
     <row r="61" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
@@ -2551,7 +2552,7 @@
       <c r="N61" s="11"/>
       <c r="O61" s="9"/>
       <c r="P61" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q61" s="7">
         <v>1</v>
@@ -2560,7 +2561,7 @@
     </row>
     <row r="62" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
@@ -2580,7 +2581,7 @@
       </c>
       <c r="O62" s="18"/>
       <c r="P62" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q62" s="7">
         <v>1</v>
@@ -2588,7 +2589,7 @@
     </row>
     <row r="63" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="18"/>
       <c r="D63" s="18"/>
@@ -2608,7 +2609,7 @@
       </c>
       <c r="O63" s="18"/>
       <c r="P63" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q63" s="7">
         <v>1</v>
@@ -2616,7 +2617,7 @@
     </row>
     <row r="64" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C64" s="18"/>
       <c r="D64" s="18"/>
@@ -2636,7 +2637,7 @@
       </c>
       <c r="O64" s="9"/>
       <c r="P64" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q64" s="7">
         <v>1</v>
@@ -2644,7 +2645,7 @@
     </row>
     <row r="65" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="18"/>
@@ -2664,16 +2665,16 @@
       </c>
       <c r="O65" s="9"/>
       <c r="P65" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q65" s="7">
-        <v>0.5</v>
+        <v>88</v>
+      </c>
+      <c r="Q65" s="26">
+        <v>1</v>
       </c>
       <c r="S65" s="45"/>
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C66" s="24"/>
       <c r="D66" s="24"/>
@@ -2693,15 +2694,15 @@
       </c>
       <c r="O66" s="9"/>
       <c r="P66" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q66" s="7">
+        <v>38</v>
+      </c>
+      <c r="Q66" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67" s="24"/>
@@ -2717,13 +2718,13 @@
       <c r="N67" s="9"/>
       <c r="O67" s="9"/>
       <c r="P67" s="10"/>
-      <c r="Q67" s="7">
-        <v>0</v>
+      <c r="Q67" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C68" s="24"/>
       <c r="D68" s="24"/>
@@ -2743,15 +2744,15 @@
         <v>25</v>
       </c>
       <c r="P68" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q68" s="7">
-        <v>0</v>
+        <v>91</v>
+      </c>
+      <c r="Q68" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C69" s="24"/>
       <c r="D69" s="24"/>
@@ -2771,15 +2772,15 @@
         <v>25</v>
       </c>
       <c r="P69" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q69" s="7">
-        <v>0</v>
+        <v>93</v>
+      </c>
+      <c r="Q69" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C70" s="24"/>
       <c r="D70" s="24"/>
@@ -2796,12 +2797,12 @@
       <c r="O70" s="18"/>
       <c r="P70" s="18"/>
       <c r="Q70" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C71" s="24"/>
       <c r="D71" s="24"/>
@@ -2819,15 +2820,15 @@
         <v>25</v>
       </c>
       <c r="P71" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q71" s="29">
-        <v>0</v>
+        <v>96</v>
+      </c>
+      <c r="Q71" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C72" s="24"/>
       <c r="D72" s="24"/>
@@ -2845,15 +2846,15 @@
         <v>25</v>
       </c>
       <c r="P72" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q72" s="29">
-        <v>0</v>
+        <v>98</v>
+      </c>
+      <c r="Q72" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C73" s="24"/>
       <c r="D73" s="24"/>
@@ -2871,15 +2872,15 @@
         <v>25</v>
       </c>
       <c r="P73" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q73" s="29">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="Q73" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C74" s="24"/>
       <c r="D74" s="24"/>
@@ -2897,15 +2898,15 @@
         <v>25</v>
       </c>
       <c r="P74" s="33" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q74" s="29">
-        <v>0</v>
+        <v>98</v>
+      </c>
+      <c r="Q74" s="26">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="37"/>
@@ -2923,15 +2924,15 @@
         <v>25</v>
       </c>
       <c r="P75" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q75" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C76" s="48"/>
       <c r="D76" s="48"/>

</xml_diff>

<commit_message>
Se actualizo el cronograma del proyecto SHS
</commit_message>
<xml_diff>
--- a/Desarrollo/SHS/Gestión/SHS-CP.xlsx
+++ b/Desarrollo/SHS/Gestión/SHS-CP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Jose Tirado\OneDrive\Escritorio\6to ciclo\PROYECTO FINAL GC\ServiceHomeStore\Desarrollo\SHS\Gestión\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8963E9CA-8080-450B-A131-A5756F1C558E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA7C3C4-2E4D-4CDF-A786-754BCC49CF85}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t>Desarrollo frontend</t>
   </si>
   <si>
-    <t>Elaborar el registro de usuarios</t>
-  </si>
-  <si>
     <t>Elaborar el login</t>
   </si>
   <si>
@@ -397,6 +394,9 @@
   </si>
   <si>
     <t>Elaboracion documento de especificación de requisitos</t>
+  </si>
+  <si>
+    <t>Elaborar el registro de usuario</t>
   </si>
 </sst>
 </file>
@@ -727,6 +727,7 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -750,7 +751,6 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -968,8 +968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AH972"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -984,46 +984,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:34" ht="18" x14ac:dyDescent="0.35">
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="52"/>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
     </row>
     <row r="2" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="53" t="s">
+      <c r="C2" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
       <c r="W2" s="2"/>
@@ -1043,67 +1043,67 @@
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="54" t="s">
+      <c r="C3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
-      <c r="K3" s="52"/>
-      <c r="L3" s="52"/>
-      <c r="M3" s="52"/>
-      <c r="N3" s="52"/>
-      <c r="O3" s="52"/>
-      <c r="P3" s="52"/>
-      <c r="Q3" s="52"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
     </row>
     <row r="4" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="56">
         <v>44132</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
-      <c r="K4" s="52"/>
-      <c r="L4" s="52"/>
-      <c r="M4" s="52"/>
-      <c r="N4" s="52"/>
-      <c r="O4" s="52"/>
-      <c r="P4" s="52"/>
-      <c r="Q4" s="52"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
+      <c r="M4" s="53"/>
+      <c r="N4" s="53"/>
+      <c r="O4" s="53"/>
+      <c r="P4" s="53"/>
+      <c r="Q4" s="53"/>
     </row>
     <row r="5" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="56">
+      <c r="C5" s="57">
         <v>44216</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="53"/>
+      <c r="N5" s="53"/>
+      <c r="O5" s="53"/>
+      <c r="P5" s="53"/>
+      <c r="Q5" s="53"/>
     </row>
     <row r="6" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -1266,28 +1266,28 @@
       </c>
     </row>
     <row r="11" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="49" t="s">
+      <c r="B11" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="50"/>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
-      <c r="J11" s="50"/>
-      <c r="K11" s="50"/>
-      <c r="L11" s="50"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="50"/>
-      <c r="O11" s="50"/>
-      <c r="P11" s="50"/>
-      <c r="Q11" s="50"/>
+      <c r="C11" s="51"/>
+      <c r="D11" s="51"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="51"/>
+      <c r="G11" s="51"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="51"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="51"/>
+      <c r="M11" s="51"/>
+      <c r="N11" s="51"/>
+      <c r="O11" s="51"/>
+      <c r="P11" s="51"/>
+      <c r="Q11" s="51"/>
     </row>
     <row r="12" spans="2:34" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B12" s="57" t="s">
-        <v>123</v>
+      <c r="B12" s="46" t="s">
+        <v>122</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
@@ -1325,7 +1325,7 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q13" s="7">
         <v>1</v>
@@ -1379,7 +1379,7 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q15" s="7">
         <v>1</v>
@@ -1407,7 +1407,7 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Q16" s="7">
         <v>1</v>
@@ -1435,7 +1435,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
       <c r="P17" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q17" s="15">
         <v>1</v>
@@ -1463,7 +1463,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Q18" s="7">
         <v>1</v>
@@ -1489,7 +1489,7 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q19" s="7">
         <v>1</v>
@@ -1515,7 +1515,7 @@
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
       <c r="P20" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q20" s="7">
         <v>1</v>
@@ -1541,7 +1541,7 @@
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
       <c r="P21" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q21" s="7">
         <v>1</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
@@ -1567,7 +1567,7 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q22" s="7">
         <v>1</v>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="23" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -1593,7 +1593,7 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q23" s="7">
         <v>1</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="24" spans="2:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1619,7 +1619,7 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q24" s="7">
         <v>1</v>
@@ -1665,7 +1665,7 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q26" s="7">
         <v>1</v>
@@ -1691,7 +1691,7 @@
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q27" s="7">
         <v>1</v>
@@ -1763,7 +1763,7 @@
       <c r="N30" s="18"/>
       <c r="O30" s="18"/>
       <c r="P30" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Q30" s="7">
         <v>1</v>
@@ -1822,24 +1822,24 @@
       </c>
     </row>
     <row r="33" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="47"/>
+      <c r="P33" s="47"/>
+      <c r="Q33" s="47"/>
     </row>
     <row r="34" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="42" t="s">
@@ -1915,7 +1915,7 @@
     </row>
     <row r="37" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>
@@ -1956,7 +1956,7 @@
     </row>
     <row r="39" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="C39" s="18"/>
       <c r="D39" s="18"/>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="40" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" s="18"/>
       <c r="D40" s="18"/>
@@ -2000,7 +2000,7 @@
       <c r="N40" s="18"/>
       <c r="O40" s="18"/>
       <c r="P40" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q40" s="7">
         <v>1</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="41" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C41" s="18"/>
       <c r="D41" s="18"/>
@@ -2034,7 +2034,7 @@
     </row>
     <row r="42" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C42" s="18"/>
       <c r="D42" s="18"/>
@@ -2056,7 +2056,7 @@
       <c r="N42" s="18"/>
       <c r="O42" s="18"/>
       <c r="P42" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q42" s="7">
         <v>1</v>
@@ -2064,7 +2064,7 @@
     </row>
     <row r="43" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C43" s="18"/>
       <c r="D43" s="18"/>
@@ -2086,7 +2086,7 @@
       <c r="N43" s="18"/>
       <c r="O43" s="18"/>
       <c r="P43" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q43" s="7">
         <v>1</v>
@@ -2094,7 +2094,7 @@
     </row>
     <row r="44" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="18"/>
@@ -2116,7 +2116,7 @@
       <c r="N44" s="18"/>
       <c r="O44" s="18"/>
       <c r="P44" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q44" s="7">
         <v>1</v>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="45" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C45" s="18"/>
       <c r="D45" s="18"/>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="46" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="C46" s="18"/>
       <c r="D46" s="18"/>
@@ -2160,7 +2160,7 @@
       <c r="N46" s="18"/>
       <c r="O46" s="18"/>
       <c r="P46" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q46" s="7">
         <v>1</v>
@@ -2168,7 +2168,7 @@
     </row>
     <row r="47" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -2184,7 +2184,7 @@
       <c r="N47" s="18"/>
       <c r="O47" s="18"/>
       <c r="P47" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Q47" s="7">
         <v>1</v>
@@ -2192,7 +2192,7 @@
     </row>
     <row r="48" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C48" s="18"/>
       <c r="D48" s="18"/>
@@ -2214,7 +2214,7 @@
       <c r="N48" s="18"/>
       <c r="O48" s="18"/>
       <c r="P48" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q48" s="7">
         <v>1</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="49" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49" s="18"/>
       <c r="D49" s="18"/>
@@ -2252,7 +2252,7 @@
     </row>
     <row r="50" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C50" s="33"/>
       <c r="D50" s="33"/>
@@ -2281,24 +2281,24 @@
       </c>
     </row>
     <row r="51" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="47" t="s">
-        <v>73</v>
-      </c>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
-      <c r="I51" s="47"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="47"/>
-      <c r="L51" s="47"/>
-      <c r="M51" s="47"/>
-      <c r="N51" s="47"/>
-      <c r="O51" s="47"/>
-      <c r="P51" s="47"/>
-      <c r="Q51" s="47"/>
+      <c r="B51" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="48"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="48"/>
+      <c r="K51" s="48"/>
+      <c r="L51" s="48"/>
+      <c r="M51" s="48"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="48"/>
+      <c r="P51" s="48"/>
+      <c r="Q51" s="48"/>
     </row>
     <row r="52" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="41" t="s">
@@ -2322,7 +2322,7 @@
     </row>
     <row r="53" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C53" s="18"/>
       <c r="D53" s="18"/>
@@ -2340,7 +2340,7 @@
       <c r="N53" s="18"/>
       <c r="O53" s="18"/>
       <c r="P53" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q53" s="7">
         <v>1</v>
@@ -2348,7 +2348,7 @@
     </row>
     <row r="54" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
@@ -2368,7 +2368,7 @@
       </c>
       <c r="O54" s="18"/>
       <c r="P54" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q54" s="7">
         <v>1</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="55" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C55" s="18"/>
       <c r="D55" s="18"/>
@@ -2396,7 +2396,7 @@
       </c>
       <c r="O55" s="18"/>
       <c r="P55" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q55" s="7">
         <v>1</v>
@@ -2404,7 +2404,7 @@
     </row>
     <row r="56" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C56" s="18"/>
       <c r="D56" s="18"/>
@@ -2424,7 +2424,7 @@
       </c>
       <c r="O56" s="18"/>
       <c r="P56" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q56" s="7">
         <v>1</v>
@@ -2432,7 +2432,7 @@
     </row>
     <row r="57" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C57" s="18"/>
       <c r="D57" s="18"/>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="O57" s="18"/>
       <c r="P57" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q57" s="7">
         <v>1</v>
@@ -2460,7 +2460,7 @@
     </row>
     <row r="58" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
@@ -2480,7 +2480,7 @@
       </c>
       <c r="O58" s="9"/>
       <c r="P58" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q58" s="7">
         <v>1</v>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="59" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C59" s="18"/>
       <c r="D59" s="18"/>
@@ -2508,7 +2508,7 @@
     </row>
     <row r="60" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60" s="18"/>
       <c r="D60" s="18"/>
@@ -2526,7 +2526,7 @@
       <c r="N60" s="11"/>
       <c r="O60" s="9"/>
       <c r="P60" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="Q60" s="7">
         <v>1</v>
@@ -2534,7 +2534,7 @@
     </row>
     <row r="61" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C61" s="18"/>
       <c r="D61" s="18"/>
@@ -2552,7 +2552,7 @@
       <c r="N61" s="11"/>
       <c r="O61" s="9"/>
       <c r="P61" s="23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="Q61" s="7">
         <v>1</v>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="62" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="O62" s="18"/>
       <c r="P62" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q62" s="7">
         <v>1</v>
@@ -2589,7 +2589,7 @@
     </row>
     <row r="63" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C63" s="18"/>
       <c r="D63" s="18"/>
@@ -2609,7 +2609,7 @@
       </c>
       <c r="O63" s="18"/>
       <c r="P63" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q63" s="7">
         <v>1</v>
@@ -2617,7 +2617,7 @@
     </row>
     <row r="64" spans="2:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C64" s="18"/>
       <c r="D64" s="18"/>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="O64" s="9"/>
       <c r="P64" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q64" s="7">
         <v>1</v>
@@ -2645,7 +2645,7 @@
     </row>
     <row r="65" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C65" s="18"/>
       <c r="D65" s="18"/>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="O65" s="9"/>
       <c r="P65" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q65" s="26">
         <v>1</v>
@@ -2674,7 +2674,7 @@
     </row>
     <row r="66" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C66" s="24"/>
       <c r="D66" s="24"/>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="67" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C67" s="24"/>
       <c r="D67" s="24"/>
@@ -2724,7 +2724,7 @@
     </row>
     <row r="68" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C68" s="24"/>
       <c r="D68" s="24"/>
@@ -2744,7 +2744,7 @@
         <v>25</v>
       </c>
       <c r="P68" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="Q68" s="26">
         <v>1</v>
@@ -2752,7 +2752,7 @@
     </row>
     <row r="69" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C69" s="24"/>
       <c r="D69" s="24"/>
@@ -2772,7 +2772,7 @@
         <v>25</v>
       </c>
       <c r="P69" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="Q69" s="26">
         <v>1</v>
@@ -2780,7 +2780,7 @@
     </row>
     <row r="70" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C70" s="24"/>
       <c r="D70" s="24"/>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="71" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C71" s="24"/>
       <c r="D71" s="24"/>
@@ -2820,7 +2820,7 @@
         <v>25</v>
       </c>
       <c r="P71" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="Q71" s="26">
         <v>1</v>
@@ -2828,7 +2828,7 @@
     </row>
     <row r="72" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C72" s="24"/>
       <c r="D72" s="24"/>
@@ -2846,7 +2846,7 @@
         <v>25</v>
       </c>
       <c r="P72" s="18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q72" s="26">
         <v>1</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="73" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C73" s="24"/>
       <c r="D73" s="24"/>
@@ -2872,7 +2872,7 @@
         <v>25</v>
       </c>
       <c r="P73" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q73" s="26">
         <v>1</v>
@@ -2880,7 +2880,7 @@
     </row>
     <row r="74" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C74" s="24"/>
       <c r="D74" s="24"/>
@@ -2898,7 +2898,7 @@
         <v>25</v>
       </c>
       <c r="P74" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Q74" s="26">
         <v>1</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="75" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C75" s="37"/>
       <c r="D75" s="37"/>
@@ -2924,31 +2924,31 @@
         <v>25</v>
       </c>
       <c r="P75" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q75" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="76" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="48" t="s">
-        <v>121</v>
-      </c>
-      <c r="C76" s="48"/>
-      <c r="D76" s="48"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="48"/>
-      <c r="G76" s="48"/>
-      <c r="H76" s="48"/>
-      <c r="I76" s="48"/>
-      <c r="J76" s="48"/>
-      <c r="K76" s="48"/>
-      <c r="L76" s="48"/>
-      <c r="M76" s="48"/>
-      <c r="N76" s="48"/>
-      <c r="O76" s="48"/>
-      <c r="P76" s="48"/>
-      <c r="Q76" s="48"/>
+      <c r="B76" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C76" s="49"/>
+      <c r="D76" s="49"/>
+      <c r="E76" s="49"/>
+      <c r="F76" s="49"/>
+      <c r="G76" s="49"/>
+      <c r="H76" s="49"/>
+      <c r="I76" s="49"/>
+      <c r="J76" s="49"/>
+      <c r="K76" s="49"/>
+      <c r="L76" s="49"/>
+      <c r="M76" s="49"/>
+      <c r="N76" s="49"/>
+      <c r="O76" s="49"/>
+      <c r="P76" s="49"/>
+      <c r="Q76" s="49"/>
     </row>
     <row r="77" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="32"/>

</xml_diff>